<commit_message>
upload data in excel file
</commit_message>
<xml_diff>
--- a/similarity/excel-master-2019-draft-similarity.xlsx
+++ b/similarity/excel-master-2019-draft-similarity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tboge\GitHub\2019-draft-ml\similarity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tboge\OneDrive\dribble-analytics\2019-draft\similarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58332B9-8457-45EE-A7EC-F26B68E3E9FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{DFB7DECC-8511-460B-90AD-C27399FB4CDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{49E3612F-F404-4DBD-9224-1652DA906236}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="3068" xr2:uid="{57C30CD0-B2C4-4823-BEBA-3EFB57F94260}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="741">
   <si>
     <t>Player</t>
   </si>
@@ -2134,9 +2134,6 @@
     <t>Data starts with the 1990 NBA draft (so that all players will have played their entire college career with a 3-point line)</t>
   </si>
   <si>
-    <t>https://dribbleanalytics.blog/2019/06/2019-draft-similarity</t>
-  </si>
-  <si>
     <t>https://github.com/dribbleanalytics/2019-draft-ml/similarity</t>
   </si>
   <si>
@@ -2255,6 +2252,9 @@
   </si>
   <si>
     <t>Generating stats-based historical comparisons for the draft lottery</t>
+  </si>
+  <si>
+    <t>https://dribbleanalytics.blog/2019/07/2019-draft-similarity</t>
   </si>
 </sst>
 </file>
@@ -2770,7 +2770,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2782,7 +2782,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.75">
       <c r="A1" s="15" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.65">
       <c r="A3" s="17" t="s">
-        <v>700</v>
+        <v>740</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -2920,7 +2920,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -3088,67 +3088,67 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>706</v>
+      </c>
+      <c r="I1" t="s">
         <v>707</v>
-      </c>
-      <c r="I1" t="s">
-        <v>708</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
       </c>
       <c r="K1" t="s">
+        <v>708</v>
+      </c>
+      <c r="L1" t="s">
         <v>709</v>
-      </c>
-      <c r="L1" t="s">
-        <v>710</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
       </c>
       <c r="N1" t="s">
+        <v>710</v>
+      </c>
+      <c r="O1" t="s">
         <v>711</v>
-      </c>
-      <c r="O1" t="s">
-        <v>712</v>
       </c>
       <c r="P1" t="s">
         <v>8</v>
       </c>
       <c r="Q1" t="s">
+        <v>712</v>
+      </c>
+      <c r="R1" t="s">
         <v>713</v>
-      </c>
-      <c r="R1" t="s">
-        <v>714</v>
       </c>
       <c r="S1" t="s">
         <v>9</v>
       </c>
       <c r="T1" t="s">
+        <v>714</v>
+      </c>
+      <c r="U1" t="s">
         <v>715</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>716</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>717</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>718</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>719</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>720</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>721</v>
       </c>
       <c r="AA1" t="s">
         <v>10</v>
@@ -3160,7 +3160,7 @@
         <v>12</v>
       </c>
       <c r="AD1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="AE1" t="s">
         <v>671</v>
@@ -3175,52 +3175,52 @@
         <v>674</v>
       </c>
       <c r="AI1" t="s">
+        <v>722</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>723</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>724</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>725</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>726</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>727</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>728</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>729</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>730</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>731</v>
       </c>
       <c r="AR1" t="s">
         <v>675</v>
       </c>
       <c r="AS1" t="s">
+        <v>731</v>
+      </c>
+      <c r="AT1" t="s">
         <v>732</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>733</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>734</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>735</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>736</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.45">
@@ -70522,67 +70522,67 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>706</v>
+      </c>
+      <c r="J1" t="s">
         <v>707</v>
-      </c>
-      <c r="J1" t="s">
-        <v>708</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
       </c>
       <c r="L1" t="s">
+        <v>708</v>
+      </c>
+      <c r="M1" t="s">
         <v>709</v>
-      </c>
-      <c r="M1" t="s">
-        <v>710</v>
       </c>
       <c r="N1" t="s">
         <v>7</v>
       </c>
       <c r="O1" t="s">
+        <v>710</v>
+      </c>
+      <c r="P1" t="s">
         <v>711</v>
-      </c>
-      <c r="P1" t="s">
-        <v>712</v>
       </c>
       <c r="Q1" t="s">
         <v>8</v>
       </c>
       <c r="R1" t="s">
+        <v>712</v>
+      </c>
+      <c r="S1" t="s">
         <v>713</v>
-      </c>
-      <c r="S1" t="s">
-        <v>714</v>
       </c>
       <c r="T1" t="s">
         <v>9</v>
       </c>
       <c r="U1" t="s">
+        <v>714</v>
+      </c>
+      <c r="V1" t="s">
         <v>715</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>716</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>717</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>718</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>719</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>720</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>721</v>
       </c>
       <c r="AB1" t="s">
         <v>10</v>
@@ -70594,7 +70594,7 @@
         <v>12</v>
       </c>
       <c r="AE1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="AF1" t="s">
         <v>671</v>
@@ -70609,52 +70609,52 @@
         <v>674</v>
       </c>
       <c r="AJ1" t="s">
+        <v>722</v>
+      </c>
+      <c r="AK1" t="s">
         <v>723</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>724</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>725</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>726</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>727</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>728</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>729</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>730</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>731</v>
       </c>
       <c r="AS1" t="s">
         <v>675</v>
       </c>
       <c r="AT1" t="s">
+        <v>731</v>
+      </c>
+      <c r="AU1" t="s">
         <v>732</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>733</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>734</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>735</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>736</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.45">
@@ -70969,7 +70969,7 @@
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -72364,7 +72364,7 @@
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B13" t="s">
         <v>108</v>

</xml_diff>